<commit_message>
Add conclusion and complete lab report 4
</commit_message>
<xml_diff>
--- a/Lab Reports/LabReport4/PHY121_Lab4_Data.xlsx
+++ b/Lab Reports/LabReport4/PHY121_Lab4_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abereni4u/Dropbox/Github/PHY121/Lab Reports/LabReport4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA061E3-A9D2-0B41-8646-58C34D2B2AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81639115-E779-7145-BA04-0D39FE5FC27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15420" windowHeight="14680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10180" yWindow="500" windowWidth="15420" windowHeight="14680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Data" sheetId="21" r:id="rId1"/>
@@ -7643,10 +7643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BEF26D-78A2-5940-94D6-EFEA168D1845}">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="A3" zoomScale="57" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8061,12 +8061,6 @@
       <c r="I24" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J24" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="K24" s="9" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
@@ -8098,14 +8092,6 @@
         <f t="shared" ref="I25:K28" si="4">TRUNC(C25, 4 - (1 + INT(LOG10(ABS(C25)))))</f>
         <v>11.22</v>
       </c>
-      <c r="J25">
-        <f t="shared" si="4"/>
-        <v>-0.53169999999999995</v>
-      </c>
-      <c r="K25">
-        <f t="shared" si="4"/>
-        <v>6.4549999999999998E-3</v>
-      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
@@ -8174,6 +8160,24 @@
       <c r="I28">
         <f t="shared" si="4"/>
         <v>14.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="G29" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29">
+        <f>TRUNC(D25, 4 - (1 + INT(LOG10(ABS(D25)))))</f>
+        <v>-0.53169999999999995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="G30" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30">
+        <f>TRUNC(E25, 4 - (1 + INT(LOG10(ABS(E25)))))</f>
+        <v>6.4549999999999998E-3</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8218,12 +8222,6 @@
       <c r="I33" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J33" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="K33" s="9" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
@@ -8255,14 +8253,6 @@
         <f t="shared" ref="I34:I37" si="7">TRUNC(C34, 4 - (1 + INT(LOG10(ABS(C34)))))</f>
         <v>8.9920000000000009</v>
       </c>
-      <c r="J34">
-        <f t="shared" ref="J34:J37" si="8">TRUNC(D34, 4 - (1 + INT(LOG10(ABS(D34)))))</f>
-        <v>-0.56430000000000002</v>
-      </c>
-      <c r="K34">
-        <f t="shared" ref="K34:K37" si="9">TRUNC(E34, 4 - (1 + INT(LOG10(ABS(E34)))))</f>
-        <v>7.1710000000000003E-3</v>
-      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
@@ -8272,14 +8262,14 @@
         <v>-0.57550000000000001</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" ref="C35:C37" si="10">ABS((B35--0.6105)/-0.6105) * 100</f>
+        <f t="shared" ref="C35:C37" si="8">ABS((B35--0.6105)/-0.6105) * 100</f>
         <v>5.7330057330057373</v>
       </c>
       <c r="G35" s="11">
         <v>2</v>
       </c>
       <c r="H35">
-        <f t="shared" ref="H35:H37" si="11">TRUNC(B35, 4 - (1 + INT(LOG10(ABS(B35)))))</f>
+        <f t="shared" ref="H35:H37" si="9">TRUNC(B35, 4 - (1 + INT(LOG10(ABS(B35)))))</f>
         <v>-0.57550000000000001</v>
       </c>
       <c r="I35">
@@ -8295,14 +8285,14 @@
         <v>-0.56220000000000003</v>
       </c>
       <c r="C36" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>7.9115479115479133</v>
       </c>
       <c r="G36" s="11">
         <v>3</v>
       </c>
       <c r="H36">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-0.56220000000000003</v>
       </c>
       <c r="I36">
@@ -8318,14 +8308,14 @@
         <v>-0.56389999999999996</v>
       </c>
       <c r="C37" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>7.6330876330876469</v>
       </c>
       <c r="G37" s="11">
         <v>4</v>
       </c>
       <c r="H37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-0.56389999999999996</v>
       </c>
       <c r="I37">
@@ -8333,94 +8323,112 @@
         <v>7.633</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="8" t="s">
+    <row r="38" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="G38" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38">
+        <f>TRUNC(D34, 4 - (1 + INT(LOG10(ABS(D34)))))</f>
+        <v>-0.56430000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="G39" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H39">
+        <f>TRUNC(E34, 4 - (1 + INT(LOG10(ABS(E34)))))</f>
+        <v>7.1710000000000003E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="G39" s="8" t="s">
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="G41" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B43" s="5">
         <v>-0.531725</v>
       </c>
-      <c r="C41" s="5">
-        <f>ABS((B41--0.6105)/-0.6105) * 100</f>
+      <c r="C43" s="5">
+        <f>ABS((B43--0.6105)/-0.6105) * 100</f>
         <v>12.903357903357909</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H41">
-        <f>TRUNC(B41, 4 - (1 + INT(LOG10(ABS(B41)))))</f>
+      <c r="H43">
+        <f>TRUNC(B43, 4 - (1 + INT(LOG10(ABS(B43)))))</f>
         <v>-0.53169999999999995</v>
       </c>
-      <c r="I41">
-        <f>TRUNC(C41, 4 - (1 + INT(LOG10(ABS(C41)))))</f>
+      <c r="I43">
+        <f>TRUNC(C43, 4 - (1 + INT(LOG10(ABS(C43)))))</f>
         <v>12.9</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="44" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B44" s="5">
         <v>-0.56430000000000002</v>
       </c>
-      <c r="C42" s="5">
-        <f>ABS((B42--0.6105)/-0.6105) * 100</f>
+      <c r="C44" s="5">
+        <f>ABS((B44--0.6105)/-0.6105) * 100</f>
         <v>7.5675675675675711</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="H42">
-        <f>TRUNC(B42, 4 - (1 + INT(LOG10(ABS(B42)))))</f>
-        <v>-0.56430000000000002</v>
-      </c>
-      <c r="I42">
-        <f>TRUNC(C42, 4 - (1 + INT(LOG10(ABS(C42)))))</f>
-        <v>7.5670000000000002</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44">
-        <v>-0.61050000000000004</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>26</v>
       </c>
       <c r="H44">
         <f>TRUNC(B44, 4 - (1 + INT(LOG10(ABS(B44)))))</f>
+        <v>-0.56430000000000002</v>
+      </c>
+      <c r="I44">
+        <f>TRUNC(C44, 4 - (1 + INT(LOG10(ABS(C44)))))</f>
+        <v>7.5670000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A46" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46">
+        <v>-0.61050000000000004</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H46">
+        <f>TRUNC(B46, 4 - (1 + INT(LOG10(ABS(B46)))))</f>
         <v>-0.61050000000000004</v>
       </c>
     </row>
@@ -8428,12 +8436,12 @@
   <mergeCells count="10">
     <mergeCell ref="A23:E23"/>
     <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A41:E41"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="G12:K12"/>
     <mergeCell ref="G23:K23"/>
     <mergeCell ref="G32:K32"/>
-    <mergeCell ref="G39:K39"/>
+    <mergeCell ref="G41:K41"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
@@ -24672,8 +24680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25099,7 +25107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" zoomScale="64" workbookViewId="0">
+    <sheetView topLeftCell="G2" zoomScale="64" workbookViewId="0">
       <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>

</xml_diff>